<commit_message>
Added validation and features
</commit_message>
<xml_diff>
--- a/Orders.xlsx
+++ b/Orders.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\Python\Ordering_System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F07D4A7-D34F-4F31-88CF-7BF6E0410753}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C34B8642-84A9-4E94-B02C-5A46CC2DD235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,12 +18,25 @@
   <definedNames>
     <definedName name="Order_ID">Orders[Order_ID]</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="35">
   <si>
     <t>Order_ID</t>
   </si>
@@ -43,6 +56,9 @@
     <t>Status</t>
   </si>
   <si>
+    <t>stats</t>
+  </si>
+  <si>
     <t>Price</t>
   </si>
   <si>
@@ -64,7 +80,7 @@
     <t>TakeOut</t>
   </si>
   <si>
-    <t>Pizza, Pizza, Carbonara, Chicken</t>
+    <t>Pizza, Pizza, Pizza, Carbonara, Carbonara, Chicken, Pancit</t>
   </si>
   <si>
     <t>Total Sales</t>
@@ -103,7 +119,28 @@
     <t>Pancit, Chicken, Pizza</t>
   </si>
   <si>
-    <t>Pizza, Pizza, Pizza, Pizza, Pizza, Pizza, Pizza, Pizza, Pizza, Pizza, Carbonara</t>
+    <t>Pizza, Pizza, Carbonara</t>
+  </si>
+  <si>
+    <t>2024-03-17</t>
+  </si>
+  <si>
+    <t>Serving</t>
+  </si>
+  <si>
+    <t>Pizza, Pizza, Lasagna</t>
+  </si>
+  <si>
+    <t>Carbonara, Carbonara, Chicken, Chicken, Chicken</t>
+  </si>
+  <si>
+    <t>Pizza, Pizza, Carbonara, Chicken, Pancit, Lasagna</t>
+  </si>
+  <si>
+    <t>Pizza, Pizza, Pizza, Carbonara, Carbonara, Carbonara, Carbonara, Carbonara, Carbonara, Carbonara, Carbonara, Carbonara, Carbonara, Chicken, Chicken, Chicken, Pancit, Pancit, Pancit, Lasagna</t>
+  </si>
+  <si>
+    <t>2024-03-18</t>
   </si>
 </sst>
 </file>
@@ -166,7 +203,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -187,102 +224,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -308,72 +249,60 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="11" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -382,117 +311,26 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Total" xfId="2" builtinId="25"/>
   </cellStyles>
-  <dxfs count="10">
-    <dxf>
-      <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
-      <alignment horizontal="center" vertical="center"/>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
+  <dxfs count="11">
     <dxf>
       <alignment horizontal="center" vertical="center"/>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="_-[$₱-3409]* #,##0.00_-;\-[$₱-3409]* #,##0.00_-;_-[$₱-3409]* &quot;-&quot;??_-;_-@_-"/>
       <alignment horizontal="center" vertical="center"/>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
     </dxf>
     <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
+      <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+      <alignment horizontal="center" vertical="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center"/>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center"/>
-      <border>
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
     </dxf>
     <dxf>
       <border outline="0">
@@ -518,6 +356,9 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
       <border outline="0">
         <bottom style="thin">
           <color indexed="64"/>
@@ -536,6 +377,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <alignment horizontal="center"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -551,8 +393,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Orders" displayName="Orders" ref="A1:F22" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
-  <autoFilter ref="A1:F22" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Orders" displayName="Orders" ref="A1:F26" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+  <autoFilter ref="A1:F26" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F22">
     <sortCondition ref="A1:A22"/>
   </sortState>
@@ -560,11 +402,11 @@
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Order_ID" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Table Number" dataDxfId="4"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Orders" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Date" dataDxfId="0"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Bill" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Status" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Date" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Bill" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Status" dataDxfId="0"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -886,82 +728,87 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.21875" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" customWidth="1"/>
-    <col min="3" max="3" width="37.109375" customWidth="1"/>
-    <col min="4" max="4" width="11.21875" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" customWidth="1"/>
-    <col min="6" max="6" width="10.88671875" customWidth="1"/>
-    <col min="8" max="8" width="12.88671875" customWidth="1"/>
-    <col min="9" max="9" width="8.88671875" customWidth="1"/>
-    <col min="10" max="10" width="14.77734375" customWidth="1"/>
-    <col min="11" max="11" width="11.21875" customWidth="1"/>
-    <col min="12" max="12" width="8.88671875" style="17" customWidth="1"/>
+    <col min="1" max="1" width="10.21875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="14.5546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="55.77734375" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.21875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="16.44140625" style="16" customWidth="1"/>
+    <col min="6" max="6" width="10.88671875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="12.88671875" style="3" customWidth="1"/>
+    <col min="9" max="9" width="8.88671875" style="3" customWidth="1"/>
+    <col min="10" max="10" width="14.77734375" style="3" customWidth="1"/>
+    <col min="11" max="11" width="11.21875" style="3" customWidth="1"/>
+    <col min="12" max="14" width="8.88671875" style="3" customWidth="1"/>
+    <col min="15" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="24" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="25" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="25" t="s">
+      <c r="J1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="25" t="s">
+      <c r="K1" s="4" t="s">
         <v>8</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="5">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="4">
+      <c r="C2" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="15">
         <v>45336</v>
       </c>
-      <c r="E2" s="15">
+      <c r="E2" s="16">
         <v>5000</v>
       </c>
-      <c r="F2" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J2" s="15">
+      <c r="F2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="7">
         <v>500</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="L2" s="16">
+      <c r="K2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" s="2">
         <v>20</v>
       </c>
     </row>
@@ -969,31 +816,31 @@
       <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="B3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="4">
+      <c r="C3" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="15">
         <v>45337</v>
       </c>
-      <c r="E3" s="3">
-        <v>500</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="J3" s="15">
+      <c r="E3" s="17">
+        <v>1300</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="7">
         <v>200</v>
       </c>
-      <c r="K3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="L3" s="16">
+      <c r="K3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L3" s="2">
         <v>18</v>
       </c>
     </row>
@@ -1001,31 +848,32 @@
       <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="5">
         <v>3</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="4">
+      <c r="C4" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="15">
         <v>45338</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="17">
         <v>4352</v>
       </c>
-      <c r="F4" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" s="14">
-        <v>45459.43</v>
-      </c>
-      <c r="J4" s="15">
+      <c r="F4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="9">
+        <f>SUM(E:E)</f>
+        <v>54200.43</v>
+      </c>
+      <c r="J4" s="7">
         <v>100</v>
       </c>
-      <c r="K4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L4" s="16">
+      <c r="K4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L4" s="2">
         <v>5</v>
       </c>
     </row>
@@ -1033,28 +881,28 @@
       <c r="A5" s="5">
         <v>4</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="5">
         <v>2</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="4">
+      <c r="C5" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="15">
         <v>45339</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="17">
         <v>1643</v>
       </c>
-      <c r="F5" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J5" s="15">
-        <v>50</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L5" s="16">
+      <c r="F5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="7">
+        <v>200</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L5" s="2">
         <v>2</v>
       </c>
     </row>
@@ -1062,28 +910,28 @@
       <c r="A6" s="5">
         <v>5</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="5">
         <v>1</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="4">
+      <c r="C6" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="15">
         <v>45340</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="17">
         <v>678</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="J6" s="15">
+      <c r="F6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J6" s="7">
         <v>300</v>
       </c>
-      <c r="K6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L6" s="16">
+      <c r="K6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L6" s="2">
         <v>3</v>
       </c>
     </row>
@@ -1091,346 +939,416 @@
       <c r="A7" s="5">
         <v>6</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="5">
         <v>2</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="4">
+      <c r="C7" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="15">
         <v>45341</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="17">
         <v>872</v>
       </c>
-      <c r="F7" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="J7" s="1"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="16"/>
+      <c r="F7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K7" s="5"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>7</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="5">
         <v>4</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="4">
+      <c r="C8" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="15">
         <v>45342</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="17">
         <v>5437</v>
       </c>
-      <c r="F8" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="J8" s="1"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="16"/>
+      <c r="F8" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K8" s="5"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>8</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="5">
         <v>8</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="4">
+      <c r="C9" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="15">
         <v>45343</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="17">
         <v>634</v>
       </c>
-      <c r="F9" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="J9" s="1"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="16"/>
+      <c r="F9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K9" s="5"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>9</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="5">
         <v>7</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="4">
+      <c r="C10" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="15">
         <v>45344</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="17">
         <v>654</v>
       </c>
-      <c r="F10" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="J10" s="1"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="16"/>
+      <c r="F10" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K10" s="5"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>10</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="5">
         <v>3</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="4">
+      <c r="C11" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="15">
         <v>45345</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="17">
         <v>134</v>
       </c>
-      <c r="F11" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="J11" s="1"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="16"/>
+      <c r="F11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K11" s="5"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>11</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="5">
         <v>4</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="4">
+      <c r="C12" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="15">
         <v>45346</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="17">
         <v>4234</v>
       </c>
-      <c r="F12" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="J12" s="1"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="16"/>
+      <c r="F12" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K12" s="5"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>12</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="5">
         <v>5</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="4">
+      <c r="C13" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="15">
         <v>45347</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="17">
         <v>543</v>
       </c>
-      <c r="F13" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="J13" s="1"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="16"/>
+      <c r="F13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K13" s="5"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>13</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="5">
         <v>6</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="4">
+      <c r="C14" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="15">
         <v>45348</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="17">
         <v>4354.43</v>
       </c>
-      <c r="F14" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="J14" s="1"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="16"/>
+      <c r="F14" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K14" s="5"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>14</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="5">
         <v>7</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D15" s="4">
+      <c r="C15" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="15">
         <v>45349</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="17">
         <v>654</v>
       </c>
-      <c r="F15" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="J15" s="1"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="16"/>
+      <c r="F15" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K15" s="5"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>15</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="5">
         <v>1</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D16" s="4">
+      <c r="C16" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="15">
         <v>45350</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="17">
         <v>234</v>
       </c>
-      <c r="F16" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="J16" s="1"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="16"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F16" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K16" s="5"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>16</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="5">
         <v>5</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" s="4">
+      <c r="C17" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="15">
         <v>45351</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E17" s="17">
         <v>53</v>
       </c>
-      <c r="F17" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="J17" s="1"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="16"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F17" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K17" s="5"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>17</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="5">
         <v>4</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D18" s="4">
+      <c r="C18" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="15">
         <v>45352</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18" s="17">
         <v>432</v>
       </c>
-      <c r="F18" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J18" s="1"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="16"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F18" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K18" s="5"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
         <v>18</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="5">
         <v>6</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D19" s="4">
+      <c r="C19" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="15">
         <v>45368</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E19" s="17">
         <v>5435</v>
       </c>
-      <c r="F19" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J19" s="1"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="16"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F19" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K19" s="5"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>19</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="5">
         <v>8</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" s="15">
+        <v>45368</v>
+      </c>
+      <c r="E20" s="17">
+        <v>543</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K20" s="5"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" s="5">
+        <v>20</v>
+      </c>
+      <c r="B21" s="5">
+        <v>7</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" s="15">
+        <v>45368</v>
+      </c>
+      <c r="E21" s="17">
+        <v>4314</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K21" s="5"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" s="5">
+        <v>23</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E22" s="17">
+        <v>4200</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" s="3">
+        <v>24</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E23" s="16">
+        <v>1300</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" s="3">
         <v>25</v>
       </c>
-      <c r="D20" s="4">
-        <v>45368</v>
-      </c>
-      <c r="E20" s="3">
-        <v>543</v>
-      </c>
-      <c r="F20" s="6" t="s">
+      <c r="B24" s="3">
+        <v>7</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E24" s="16">
+        <v>700</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" s="5">
+        <v>26</v>
+      </c>
+      <c r="B25" s="5">
+        <v>7</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25" s="17">
+        <v>1800</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" s="5">
+        <v>27</v>
+      </c>
+      <c r="B26" s="5">
         <v>10</v>
       </c>
-      <c r="J20" s="1"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="16"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A21" s="7">
-        <v>20</v>
-      </c>
-      <c r="B21" s="8">
-        <v>7</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D21" s="10">
-        <v>45368</v>
-      </c>
-      <c r="E21" s="11">
-        <v>4314</v>
-      </c>
-      <c r="F21" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="J21" s="1"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="16"/>
+      <c r="C26" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E26" s="17">
+        <v>4700</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>29</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="5">
@@ -1441,13 +1359,13 @@
       <formula1>44927</formula1>
       <formula2>45658</formula2>
     </dataValidation>
-    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" sqref="D2:D22" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" sqref="D2:D26" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>45336</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F2:F22" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F2:F26" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"Serving, Pending, Dining, Completed"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B2:B22" xr:uid="{00000000-0002-0000-0000-000004000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B2:B26" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>"1,2,3,4,5,6,7,8,9,10,TakeOut"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>